<commit_message>
Clarify text in PCBs
O Add text for 3PDT Switch breakout board better PCB annotation
O Rename MOSFET that controls LED for Programming Mode -> P_MOS
+ Add JST Male to BOM Logic Module – Power V8
O Correct excel formula for a total price of Logic Module
</commit_message>
<xml_diff>
--- a/Hardware/Electrical Components/Module - Logic/BOM Logic Module - Power V8.xlsx
+++ b/Hardware/Electrical Components/Module - Logic/BOM Logic Module - Power V8.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91363FE6-8E0A-4577-8DA9-D4C57AAA1637}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C319FC3-57D8-4D48-BA5A-4534BB618BD3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="60">
   <si>
     <t>Link</t>
   </si>
@@ -181,9 +181,6 @@
     <t>BSS84-FDICT-ND</t>
   </si>
   <si>
-    <t>JST Connector 5POS 2.5mm</t>
-  </si>
-  <si>
     <t>455-2270-ND</t>
   </si>
   <si>
@@ -197,6 +194,18 @@
   </si>
   <si>
     <t>HDR100IMP40M-G-RA-TH-ND</t>
+  </si>
+  <si>
+    <t>5mm LED</t>
+  </si>
+  <si>
+    <t>JST Connector 5POS 2.5mm Female</t>
+  </si>
+  <si>
+    <t>JST Connector 5POS 2.5mm Male</t>
+  </si>
+  <si>
+    <t>455-2268-ND</t>
   </si>
 </sst>
 </file>
@@ -206,7 +215,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +258,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -273,7 +289,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -296,6 +312,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -579,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:P28"/>
+  <dimension ref="B1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,7 +666,7 @@
       </c>
       <c r="M3" s="6"/>
       <c r="N3" s="6">
-        <f t="shared" ref="N3:N17" si="0">I3*L3</f>
+        <f t="shared" ref="N3:N19" si="0">I3*L3</f>
         <v>34.950000000000003</v>
       </c>
     </row>
@@ -777,42 +794,24 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="10" t="s">
+    <row r="8" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="4">
-        <v>1</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" s="7">
-        <v>0.79</v>
-      </c>
-      <c r="M8" s="7"/>
-      <c r="N8" s="6">
-        <f t="shared" si="0"/>
-        <v>0.79</v>
-      </c>
-      <c r="P8" t="s">
-        <v>5</v>
-      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="12"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -820,9 +819,9 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="I9">
+        <v>55</v>
+      </c>
+      <c r="I9" s="4">
         <v>1</v>
       </c>
       <c r="J9" s="5" t="s">
@@ -831,20 +830,21 @@
       <c r="K9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="M9" s="4">
-        <v>0.25</v>
-      </c>
+      <c r="L9" s="7">
+        <v>0.79</v>
+      </c>
+      <c r="M9" s="7"/>
       <c r="N9" s="6">
         <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.79</v>
+      </c>
+      <c r="P9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -852,71 +852,67 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="I10" s="5">
+        <v>51</v>
+      </c>
+      <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="L10" s="5">
-        <v>3.04</v>
-      </c>
-      <c r="M10" s="5">
-        <v>3.04</v>
+        <v>8</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0.25</v>
       </c>
       <c r="N10" s="6">
         <f t="shared" si="0"/>
-        <v>3.04</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="11" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
-      <c r="H11" s="10" t="s">
-        <v>44</v>
+      <c r="H11" s="18" t="s">
+        <v>59</v>
       </c>
       <c r="I11" s="5">
         <v>1</v>
       </c>
-      <c r="J11" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="K11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="L11" s="5">
-        <v>0.28999999999999998</v>
+        <v>0.12</v>
       </c>
       <c r="M11" s="5">
-        <v>0.28999999999999998</v>
+        <v>0.12</v>
       </c>
       <c r="N11" s="6">
-        <f t="shared" si="0"/>
-        <v>0.28999999999999998</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="12" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
-      <c r="H12" s="12" t="s">
-        <v>35</v>
+      <c r="H12" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="I12" s="5">
         <v>1</v>
@@ -924,23 +920,23 @@
       <c r="J12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K12" s="11" t="s">
         <v>4</v>
       </c>
       <c r="L12" s="5">
-        <v>0.51</v>
+        <v>3.04</v>
       </c>
       <c r="M12" s="5">
-        <v>0.51</v>
+        <v>3.04</v>
       </c>
       <c r="N12" s="6">
         <f t="shared" si="0"/>
-        <v>0.51</v>
+        <v>3.04</v>
       </c>
     </row>
     <row r="13" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="15" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -948,7 +944,7 @@
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
       <c r="H13" s="10" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I13" s="5">
         <v>1</v>
@@ -956,52 +952,55 @@
       <c r="J13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="14" t="s">
+      <c r="K13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="L13" s="5">
-        <v>2.25</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="M13" s="5">
-        <v>2.25</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="N13" s="6">
         <f t="shared" si="0"/>
-        <v>2.25</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="14" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="15" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
-      <c r="H14" s="10" t="s">
-        <v>33</v>
+      <c r="H14" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="I14" s="5">
         <v>1</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K14" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="L14" s="5">
-        <v>0.11</v>
+        <v>0.51</v>
+      </c>
+      <c r="M14" s="5">
+        <v>0.51</v>
       </c>
       <c r="N14" s="6">
         <f t="shared" si="0"/>
-        <v>0.11</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="15" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1009,7 +1008,7 @@
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="10" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="I15" s="5">
         <v>1</v>
@@ -1017,20 +1016,23 @@
       <c r="J15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="K15" s="14" t="s">
         <v>4</v>
       </c>
       <c r="L15" s="5">
-        <v>1.44</v>
+        <v>2.25</v>
+      </c>
+      <c r="M15" s="5">
+        <v>2.25</v>
       </c>
       <c r="N15" s="6">
         <f t="shared" si="0"/>
-        <v>1.44</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="16" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -1038,34 +1040,28 @@
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I16" s="5">
         <v>1</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K16" s="13" t="s">
         <v>4</v>
       </c>
       <c r="L16" s="5">
-        <v>0.62</v>
-      </c>
-      <c r="M16" s="5">
-        <v>0.62</v>
+        <v>0.11</v>
       </c>
       <c r="N16" s="6">
         <f t="shared" si="0"/>
-        <v>0.62</v>
-      </c>
-      <c r="P16" s="5" t="s">
-        <v>42</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="17" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="15" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -1073,7 +1069,7 @@
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="10" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="I17" s="5">
         <v>1</v>
@@ -1085,152 +1081,217 @@
         <v>4</v>
       </c>
       <c r="L17" s="5">
-        <v>0.66</v>
-      </c>
-      <c r="M17" s="5">
-        <v>0.66</v>
+        <v>1.44</v>
       </c>
       <c r="N17" s="6">
         <f t="shared" si="0"/>
-        <v>0.66</v>
-      </c>
-      <c r="P17" s="5" t="s">
-        <v>43</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="18" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="15" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
-      <c r="H18" s="5" t="s">
-        <v>26</v>
+      <c r="H18" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I18" s="5">
         <v>1</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>4</v>
       </c>
       <c r="L18" s="5">
-        <v>1.38</v>
+        <v>0.62</v>
       </c>
       <c r="M18" s="5">
-        <v>1.38</v>
-      </c>
-      <c r="N18" s="5">
-        <v>1.38</v>
+        <v>0.62</v>
+      </c>
+      <c r="N18" s="6">
+        <f t="shared" si="0"/>
+        <v>0.62</v>
+      </c>
+      <c r="P18" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
+      <c r="H19" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="I19" s="5">
         <v>1</v>
       </c>
-      <c r="K19" s="1"/>
+      <c r="J19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L19" s="5">
+        <v>0.66</v>
+      </c>
+      <c r="M19" s="5">
+        <v>0.66</v>
+      </c>
       <c r="N19" s="6">
+        <f t="shared" si="0"/>
+        <v>0.66</v>
+      </c>
+      <c r="P19" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="5">
+        <v>1</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L20" s="5">
+        <v>1.38</v>
+      </c>
+      <c r="M20" s="5">
+        <v>1.38</v>
+      </c>
+      <c r="N20" s="5">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="I21" s="5">
+        <v>1</v>
+      </c>
+      <c r="K21" s="1"/>
+      <c r="N21" s="6">
         <f>38.5/3</f>
         <v>12.833333333333334</v>
       </c>
     </row>
-    <row r="20" spans="2:16" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="M22" s="4" t="s">
+    <row r="22" spans="2:16" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="M24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N22" s="2">
-        <f ca="1">SUM(N3:N24)</f>
-        <v>63.568333333333328</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H24" s="10"/>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I25" s="1"/>
+      <c r="N24" s="2">
+        <f>SUM(N3:N21)</f>
+        <v>60.633333333333326</v>
+      </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="H26" s="10"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="1"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
         <v>20</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:N9">
-    <sortCondition ref="J3:J9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:N10">
+    <sortCondition ref="J3:J10"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="K8" r:id="rId1" xr:uid="{C84E417E-1A05-4EA8-A9BC-90C6F4C63514}"/>
+    <hyperlink ref="K9" r:id="rId1" xr:uid="{C84E417E-1A05-4EA8-A9BC-90C6F4C63514}"/>
     <hyperlink ref="K4" r:id="rId2" xr:uid="{B6C16CEB-3B62-4525-A163-D00A0FAE5AFF}"/>
     <hyperlink ref="K7" r:id="rId3" xr:uid="{0EFADCA7-279A-4408-A213-236D94739BAD}"/>
     <hyperlink ref="K3" r:id="rId4" xr:uid="{4F14628E-DF40-4419-B9D6-804A1E0976AE}"/>
-    <hyperlink ref="G25" r:id="rId5" xr:uid="{33898DA6-502C-48EE-B4CE-423818331D28}"/>
-    <hyperlink ref="H25" r:id="rId6" xr:uid="{EC50F461-D730-4F55-B7F8-92425D26D533}"/>
-    <hyperlink ref="G26" r:id="rId7" xr:uid="{D3B2FC3A-75B4-4C5F-994D-3753538F0CA9}"/>
-    <hyperlink ref="G28" r:id="rId8" xr:uid="{4BE09FA3-85E6-4252-A72A-945F4EDAFD50}"/>
-    <hyperlink ref="G27" r:id="rId9" xr:uid="{A0CB18FF-1281-45EE-92E3-4BF838EF1042}"/>
-    <hyperlink ref="K18" r:id="rId10" xr:uid="{BC48628A-656C-4AE2-8D43-45DCCBAC5C34}"/>
-    <hyperlink ref="K10" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="K14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="K13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="K12" r:id="rId14" xr:uid="{0D4C4276-ECE4-4878-86AC-36C1328ACD6D}"/>
-    <hyperlink ref="K15" r:id="rId15" xr:uid="{1DE7226F-2870-4E8F-A9B5-D2F2964D17F0}"/>
-    <hyperlink ref="K16" r:id="rId16" xr:uid="{432A9724-1D04-4A91-8632-324D1D6EE22F}"/>
-    <hyperlink ref="K17" r:id="rId17" xr:uid="{E5CC584D-53DE-483E-A769-5FB972607FD1}"/>
-    <hyperlink ref="K11" r:id="rId18" xr:uid="{6D627576-B046-4525-BF27-80E3C6A5DEFC}"/>
+    <hyperlink ref="G27" r:id="rId5" xr:uid="{33898DA6-502C-48EE-B4CE-423818331D28}"/>
+    <hyperlink ref="H27" r:id="rId6" xr:uid="{EC50F461-D730-4F55-B7F8-92425D26D533}"/>
+    <hyperlink ref="G28" r:id="rId7" xr:uid="{D3B2FC3A-75B4-4C5F-994D-3753538F0CA9}"/>
+    <hyperlink ref="G30" r:id="rId8" xr:uid="{4BE09FA3-85E6-4252-A72A-945F4EDAFD50}"/>
+    <hyperlink ref="G29" r:id="rId9" xr:uid="{A0CB18FF-1281-45EE-92E3-4BF838EF1042}"/>
+    <hyperlink ref="K20" r:id="rId10" xr:uid="{BC48628A-656C-4AE2-8D43-45DCCBAC5C34}"/>
+    <hyperlink ref="K12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="K15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="K14" r:id="rId14" xr:uid="{0D4C4276-ECE4-4878-86AC-36C1328ACD6D}"/>
+    <hyperlink ref="K17" r:id="rId15" xr:uid="{1DE7226F-2870-4E8F-A9B5-D2F2964D17F0}"/>
+    <hyperlink ref="K18" r:id="rId16" xr:uid="{432A9724-1D04-4A91-8632-324D1D6EE22F}"/>
+    <hyperlink ref="K19" r:id="rId17" xr:uid="{E5CC584D-53DE-483E-A769-5FB972607FD1}"/>
+    <hyperlink ref="K13" r:id="rId18" xr:uid="{6D627576-B046-4525-BF27-80E3C6A5DEFC}"/>
     <hyperlink ref="K6" r:id="rId19" xr:uid="{EFC5EBC2-8EAA-4378-BDDC-7978240F05BF}"/>
     <hyperlink ref="K5" r:id="rId20" xr:uid="{A59D24A5-CE93-49B4-B16D-C18951110374}"/>
-    <hyperlink ref="K9" r:id="rId21" xr:uid="{E4688478-3C6C-46AA-B8D1-9AEF9A188317}"/>
-    <hyperlink ref="G24" r:id="rId22" xr:uid="{C062712D-18D1-4784-B1D5-220F73D313B8}"/>
+    <hyperlink ref="K10" r:id="rId21" xr:uid="{E4688478-3C6C-46AA-B8D1-9AEF9A188317}"/>
+    <hyperlink ref="G26" r:id="rId22" xr:uid="{C062712D-18D1-4784-B1D5-220F73D313B8}"/>
+    <hyperlink ref="K11" r:id="rId23" display="https://www.digikey.com/product-detail/en/jst-sales-america-inc/XHP-5/455-2268-ND/1125486" xr:uid="{38EE6EC7-66A2-4AB9-B68C-6E74A8CB4737}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>